<commit_message>
added 1988 Montana & Missouri
</commit_message>
<xml_diff>
--- a/Output/1988/Arkansas/Arkansas.xlsx
+++ b/Output/1988/Arkansas/Arkansas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3992" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3991" uniqueCount="495">
   <si>
     <t>State</t>
   </si>
@@ -5482,8 +5482,8 @@
       <c r="L49">
         <v>17</v>
       </c>
-      <c r="M49" t="s">
-        <v>30</v>
+      <c r="M49">
+        <v>23</v>
       </c>
       <c r="N49">
         <v>41</v>

</xml_diff>